<commit_message>
Upload new challenge files with proper metadata
</commit_message>
<xml_diff>
--- a/Challenge2AnswerTemplate.xlsx
+++ b/Challenge2AnswerTemplate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2316" windowWidth="13116" windowHeight="9636" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2652" windowWidth="13116" windowHeight="9636" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="40">
   <si>
     <t>Pad ID</t>
   </si>
@@ -981,10 +981,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1198,7 +1198,7 @@
     </row>
     <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10" s="5">
         <v>1</v>
@@ -1220,7 +1220,7 @@
     </row>
     <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B11" s="5">
         <v>1</v>
@@ -1242,7 +1242,7 @@
     </row>
     <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B12" s="3">
         <v>1</v>
@@ -1264,7 +1264,7 @@
     </row>
     <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B13" s="3">
         <v>1</v>
@@ -1286,13 +1286,13 @@
     </row>
     <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B14" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="5">
-        <v>0.1</v>
+        <v>1.5</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>36</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B15" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" s="5">
-        <v>0.1</v>
+        <v>1.5</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>37</v>
@@ -1330,7 +1330,7 @@
     </row>
     <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B16" s="2">
         <v>2</v>
@@ -1352,7 +1352,7 @@
     </row>
     <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B17" s="2">
         <v>2</v>
@@ -1374,7 +1374,7 @@
     </row>
     <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B18" s="4">
         <v>2</v>
@@ -1396,7 +1396,7 @@
     </row>
     <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B19" s="4">
         <v>2</v>
@@ -1418,7 +1418,7 @@
     </row>
     <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B20" s="3">
         <v>2</v>
@@ -1440,7 +1440,7 @@
     </row>
     <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B21" s="3">
         <v>2</v>
@@ -1462,13 +1462,13 @@
     </row>
     <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B22" s="5">
         <v>2</v>
       </c>
       <c r="C22" s="5">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>36</v>
@@ -1484,13 +1484,13 @@
     </row>
     <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B23" s="5">
         <v>2</v>
       </c>
       <c r="C23" s="5">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>37</v>
@@ -1506,13 +1506,13 @@
     </row>
     <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B24" s="3">
         <v>2</v>
       </c>
       <c r="C24" s="3">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>36</v>
@@ -1528,13 +1528,13 @@
     </row>
     <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B25" s="3">
         <v>2</v>
       </c>
       <c r="C25" s="3">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>37</v>
@@ -1550,13 +1550,13 @@
     </row>
     <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B26" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C26" s="5">
-        <v>1.5</v>
+        <v>5</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>36</v>
@@ -1572,13 +1572,13 @@
     </row>
     <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B27" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C27" s="5">
-        <v>1.5</v>
+        <v>5</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>37</v>
@@ -1594,7 +1594,7 @@
     </row>
     <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B28" s="2">
         <v>3</v>
@@ -1616,7 +1616,7 @@
     </row>
     <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B29" s="2">
         <v>3</v>
@@ -1638,7 +1638,7 @@
     </row>
     <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B30" s="4">
         <v>3</v>
@@ -1660,7 +1660,7 @@
     </row>
     <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B31" s="4">
         <v>3</v>
@@ -1682,13 +1682,13 @@
     </row>
     <row r="32" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B32" s="3">
         <v>3</v>
       </c>
       <c r="C32" s="3">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>36</v>
@@ -1704,13 +1704,13 @@
     </row>
     <row r="33" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B33" s="3">
         <v>3</v>
       </c>
       <c r="C33" s="3">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>37</v>
@@ -1726,13 +1726,13 @@
     </row>
     <row r="34" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B34" s="5">
         <v>3</v>
       </c>
       <c r="C34" s="5">
-        <v>1.5</v>
+        <v>7.5</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>36</v>
@@ -1748,13 +1748,13 @@
     </row>
     <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B35" s="5">
         <v>3</v>
       </c>
       <c r="C35" s="5">
-        <v>1.5</v>
+        <v>7.5</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>37</v>
@@ -1768,60 +1768,16 @@
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
     </row>
-    <row r="36" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B36" s="3">
-        <v>3</v>
-      </c>
-      <c r="C36" s="3">
-        <v>7.5</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-    </row>
-    <row r="37" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" s="3">
-        <v>3</v>
-      </c>
-      <c r="C37" s="3">
-        <v>7.5</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E41" s="16"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E42" s="16"/>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E39" s="16"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E40" s="16"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
-    <protectedRange sqref="E4:L37" name="Range1"/>
+    <protectedRange sqref="E4:L35" name="Range1"/>
   </protectedRanges>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>